<commit_message>
deleted:    Cage No108.csv 	deleted:    Cage No65.csv 	deleted:    Cage No776.csv 	deleted:    Cage No78.csv 	modified:   Test.xlsx
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TRIMBLE\Desktop\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15199F92-AD40-4092-A2A7-2AC71290EA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE922F42-21C9-48E6-850F-5EFF0127BFB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2472" yWindow="2472" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="28">
   <si>
     <t>Cage No.</t>
   </si>
@@ -166,6 +166,21 @@
     <t>TDFL STRT</t>
   </si>
   <si>
+    <t>https://github.com/RothwellMS/Storage/blob/main/Cage%20No108.csv</t>
+  </si>
+  <si>
+    <t>https://github.com/RothwellMS/Storage/blob/main/Cage%20No78.csv</t>
+  </si>
+  <si>
+    <t>https://github.com/RothwellMS/Storage/blob/main/Cage%20No65.csv</t>
+  </si>
+  <si>
+    <t>https://github.com/RothwellMS/Storage/blob/main/Cage%20No776.csv</t>
+  </si>
+  <si>
+    <t>https://github.com/RothwellMS/Storage/blob/main/Cage%20No6.csv</t>
+  </si>
+  <si>
     <t>PITT</t>
   </si>
   <si>
@@ -179,6 +194,9 @@
   </si>
   <si>
     <t>T-Taper</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1325,7 +1343,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>967001</v>
@@ -1337,7 +1355,7 @@
         <v>62</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1415,10 +1433,10 @@
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1519,7 +1537,7 @@
         <v>223</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1882,10 +1900,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="A4" sqref="A4:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1951,6 +1969,11 @@
         <v>16</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E1" location="Title!A1" display="Click here to return" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
@@ -2717,7 +2740,7 @@
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <sheetPr codeName="Sheet17"/>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
@@ -2763,6 +2786,31 @@
         <v>12</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E1" location="Title!A1" display="Click here to return" xr:uid="{00000000-0004-0000-1F00-000000000000}"/>

</xml_diff>